<commit_message>
Update NFL injury graphs to 2019
</commit_message>
<xml_diff>
--- a/nfl/injury data/InjuryData.xlsx
+++ b/nfl/injury data/InjuryData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\nuffle\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adam\PycharmProjects\data_analysis\nfl\injury data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8899604-435D-4EF8-818C-F85854AD53A3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4B7F720-C225-422B-B795-5D8B1244308C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2628" windowWidth="10800" windowHeight="7344" firstSheet="1" activeTab="2" xr2:uid="{6532263B-0B42-498D-AD4A-82AFD2386EA3}"/>
   </bookViews>
@@ -411,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{397599AA-04AE-4685-B8D7-79248ECAEEFC}">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A2"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -517,7 +517,7 @@
         <v>38</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:D9" si="0">B4+C4</f>
+        <f t="shared" ref="D4:D10" si="0">B4+C4</f>
         <v>77</v>
       </c>
       <c r="E4">
@@ -527,19 +527,19 @@
         <v>148</v>
       </c>
       <c r="G4">
-        <f t="shared" ref="G4:G9" si="1">F4+E4</f>
+        <f t="shared" ref="G4:G10" si="1">F4+E4</f>
         <v>152</v>
       </c>
       <c r="H4">
-        <f t="shared" ref="H4:H9" si="2">E4+B4</f>
+        <f t="shared" ref="H4:H10" si="2">E4+B4</f>
         <v>43</v>
       </c>
       <c r="I4">
-        <f t="shared" ref="I4:I9" si="3">F4+C4</f>
+        <f t="shared" ref="I4:I10" si="3">F4+C4</f>
         <v>186</v>
       </c>
       <c r="J4">
-        <f t="shared" ref="J4:J9" si="4">I4+H4</f>
+        <f t="shared" ref="J4:J10" si="4">I4+H4</f>
         <v>229</v>
       </c>
     </row>
@@ -726,6 +726,43 @@
       <c r="J9">
         <f t="shared" si="4"/>
         <v>214</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>2019</v>
+      </c>
+      <c r="B10">
+        <v>30</v>
+      </c>
+      <c r="C10">
+        <v>49</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>79</v>
+      </c>
+      <c r="E10">
+        <v>9</v>
+      </c>
+      <c r="F10">
+        <v>136</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="1"/>
+        <v>145</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="2"/>
+        <v>39</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="3"/>
+        <v>185</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="4"/>
+        <v>224</v>
       </c>
     </row>
   </sheetData>
@@ -741,10 +778,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B474D171-490D-4A0D-A68A-521A17262C3B}">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -847,7 +884,7 @@
         <v>10</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:D9" si="0">B4+C4</f>
+        <f t="shared" ref="D4:D10" si="0">B4+C4</f>
         <v>25</v>
       </c>
       <c r="E4">
@@ -857,11 +894,11 @@
         <v>33</v>
       </c>
       <c r="G4">
-        <f t="shared" ref="G4:G9" si="1">F4+E4</f>
+        <f t="shared" ref="G4:G10" si="1">F4+E4</f>
         <v>36</v>
       </c>
       <c r="H4">
-        <f t="shared" ref="H4:I9" si="2">E4+B4</f>
+        <f t="shared" ref="H4:I10" si="2">E4+B4</f>
         <v>18</v>
       </c>
       <c r="I4">
@@ -869,7 +906,7 @@
         <v>43</v>
       </c>
       <c r="J4">
-        <f t="shared" ref="J4:J9" si="3">I4+H4</f>
+        <f t="shared" ref="J4:J10" si="3">I4+H4</f>
         <v>61</v>
       </c>
     </row>
@@ -1056,6 +1093,43 @@
       <c r="J9">
         <f t="shared" si="3"/>
         <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>2019</v>
+      </c>
+      <c r="B10">
+        <v>7</v>
+      </c>
+      <c r="C10">
+        <v>10</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="E10">
+        <v>7</v>
+      </c>
+      <c r="F10">
+        <v>23</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="2"/>
+        <v>33</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="3"/>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1071,10 +1145,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEC63A0E-AAF0-4610-8596-824AD5B68813}">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1177,7 +1251,7 @@
         <v>25</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:D9" si="0">B4+C4</f>
+        <f t="shared" ref="D4:D10" si="0">B4+C4</f>
         <v>45</v>
       </c>
       <c r="E4">
@@ -1187,11 +1261,11 @@
         <v>85</v>
       </c>
       <c r="G4">
-        <f t="shared" ref="G4:G9" si="1">F4+E4</f>
+        <f t="shared" ref="G4:G10" si="1">F4+E4</f>
         <v>89</v>
       </c>
       <c r="H4">
-        <f t="shared" ref="H4:I9" si="2">E4+B4</f>
+        <f t="shared" ref="H4:I10" si="2">E4+B4</f>
         <v>24</v>
       </c>
       <c r="I4">
@@ -1199,7 +1273,7 @@
         <v>110</v>
       </c>
       <c r="J4">
-        <f t="shared" ref="J4:J9" si="3">I4+H4</f>
+        <f t="shared" ref="J4:J10" si="3">I4+H4</f>
         <v>134</v>
       </c>
     </row>
@@ -1386,6 +1460,43 @@
       <c r="J9">
         <f t="shared" si="3"/>
         <v>131</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>2019</v>
+      </c>
+      <c r="B10">
+        <v>7</v>
+      </c>
+      <c r="C10">
+        <v>23</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="E10">
+        <v>3</v>
+      </c>
+      <c r="F10">
+        <v>76</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="1"/>
+        <v>79</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="2"/>
+        <v>99</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="3"/>
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>